<commit_message>
20 setting up run modes
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/TestData.xlsx
+++ b/src/test/resources/excel/TestData.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="addCustomerTest" sheetId="1" r:id="rId1"/>
-    <sheet name="openAccountTest" sheetId="2" r:id="rId2"/>
+    <sheet name="TestSuite" sheetId="3" r:id="rId2"/>
+    <sheet name="openAccountTest" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>FirstName</t>
   </si>
@@ -44,7 +45,46 @@
     <t>Currency</t>
   </si>
   <si>
-    <t>Rupees</t>
+    <t>Radha Raman</t>
+  </si>
+  <si>
+    <t>Rupee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Account created successfully with account Number </t>
+  </si>
+  <si>
+    <t>Madhusudan</t>
+  </si>
+  <si>
+    <t>Rasbihari</t>
+  </si>
+  <si>
+    <t>Govinda</t>
+  </si>
+  <si>
+    <t>Gopal</t>
+  </si>
+  <si>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>RUNMODE</t>
+  </si>
+  <si>
+    <t>AddCustomerTest</t>
+  </si>
+  <si>
+    <t>LoginTest</t>
+  </si>
+  <si>
+    <t>OpenAccountTest</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -80,8 +120,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,42 +429,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="1" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="26.28515625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>354356</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1">
+        <v>354357</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1">
+        <v>354358</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1">
+        <v>354359</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -432,28 +519,90 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="10.42578125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>